<commit_message>
desafio1 normatizacao e ciacao do banco
</commit_message>
<xml_diff>
--- a/SpotifyClone-Non-NormalizedTable.xlsx
+++ b/SpotifyClone-Non-NormalizedTable.xlsx
@@ -1,17 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TRYBE\Git\sd-07-mysql-one-for-all\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="40" windowWidth="15960" windowHeight="18080"/>
+    <workbookView xWindow="0" yWindow="36" windowWidth="15960" windowHeight="18084" activeTab="3"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="1ª" sheetId="7" r:id="rId2"/>
+    <sheet name="2ª" sheetId="9" r:id="rId3"/>
+    <sheet name="3ª" sheetId="8" r:id="rId4"/>
   </sheets>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="63">
   <si>
     <t>usuario_id</t>
   </si>
@@ -128,39 +139,111 @@
   </si>
   <si>
     <t>"Thang Of Thunder", "Words Of Her Life", "Without My Streets"</t>
+  </si>
+  <si>
+    <t>Magic Circus</t>
+  </si>
+  <si>
+    <t>Diamond Power</t>
+  </si>
+  <si>
+    <t>Thang Of Thunder</t>
+  </si>
+  <si>
+    <t>Soul For Us</t>
+  </si>
+  <si>
+    <t>Home Forever</t>
+  </si>
+  <si>
+    <t>Words Of Her Life</t>
+  </si>
+  <si>
+    <t>Reflections Of Magic</t>
+  </si>
+  <si>
+    <t>Honey, Let's Be Silly</t>
+  </si>
+  <si>
+    <t>Dance With Her Own</t>
+  </si>
+  <si>
+    <t>Without My Streets</t>
+  </si>
+  <si>
+    <t>Celebration Of More</t>
+  </si>
+  <si>
+    <t>Troubles Of My Inner Fire</t>
+  </si>
+  <si>
+    <t>Time Fireworks</t>
+  </si>
+  <si>
+    <t>Honey, So Do I</t>
+  </si>
+  <si>
+    <t>Sweetie, Let's Go Wild</t>
+  </si>
+  <si>
+    <t>She Knows</t>
+  </si>
+  <si>
+    <t>Rock His Everything</t>
+  </si>
+  <si>
+    <t>Fantasy For Me</t>
+  </si>
+  <si>
+    <t>plano_id</t>
+  </si>
+  <si>
+    <t>artista_id</t>
+  </si>
+  <si>
+    <t>seguindo_artista_id</t>
+  </si>
+  <si>
+    <t>cancao</t>
+  </si>
+  <si>
+    <t>cancao_id</t>
+  </si>
+  <si>
+    <t>seguindo_artista</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="0" formatCode="General"/>
-  </numFmts>
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
       <name val="Calibri"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color indexed="8"/>
-      <name val="Helvetica Neue"/>
-    </font>
-    <font>
-      <sz val="14"/>
-      <color indexed="8"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <b val="1"/>
+      <b/>
       <sz val="11"/>
       <color indexed="9"/>
       <name val="Calibri"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color indexed="9"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -185,8 +268,20 @@
         <bgColor auto="1"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="13">
+  <borders count="23">
     <border>
       <left/>
       <right/>
@@ -362,96 +457,371 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="12"/>
+      </right>
+      <top style="thin">
+        <color indexed="11"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="11"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="12"/>
+      </left>
+      <right style="thin">
+        <color indexed="12"/>
+      </right>
+      <top style="thin">
+        <color indexed="11"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="11"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="11"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="11"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="12"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="11"/>
+      </left>
+      <right style="thin">
+        <color indexed="12"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="12"/>
+      </left>
+      <right style="thin">
+        <color indexed="11"/>
+      </right>
+      <top style="thin">
+        <color indexed="11"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="12"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="11"/>
+      </left>
+      <right style="thin">
+        <color theme="3"/>
+      </right>
+      <top style="thin">
+        <color indexed="11"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="11"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="3"/>
+      </left>
+      <right style="thin">
+        <color theme="3"/>
+      </right>
+      <top style="thin">
+        <color indexed="11"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="11"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="3"/>
+      </left>
+      <right style="thin">
+        <color indexed="11"/>
+      </right>
+      <top style="thin">
+        <color indexed="11"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="11"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
-    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+  <cellXfs count="91">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="11" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="10" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="6" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="6" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="4" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="5" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="5" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="5" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="5" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="2" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="2" fillId="4" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -461,27 +831,85 @@
   <tableStyles count="0"/>
   <colors>
     <indexedColors>
-      <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="ffffffff"/>
-      <rgbColor rgb="ffff0000"/>
-      <rgbColor rgb="ff00ff00"/>
-      <rgbColor rgb="ff0000ff"/>
-      <rgbColor rgb="ffffff00"/>
-      <rgbColor rgb="ffff00ff"/>
-      <rgbColor rgb="ff00ffff"/>
-      <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="ffffffff"/>
-      <rgbColor rgb="ff4472c4"/>
-      <rgbColor rgb="ff8eaadb"/>
-      <rgbColor rgb="ffaaaaaa"/>
-      <rgbColor rgb="ffd9e2f3"/>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FF4472C4"/>
+      <rgbColor rgb="FF8EAADB"/>
+      <rgbColor rgb="FFAAAAAA"/>
+      <rgbColor rgb="FFD9E2F3"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office Theme">
       <a:dk1>
@@ -683,7 +1111,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -702,7 +1130,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1100" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -732,7 +1160,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -758,7 +1186,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -784,7 +1212,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -810,7 +1238,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -836,7 +1264,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -862,7 +1290,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -888,7 +1316,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -914,7 +1342,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -940,7 +1368,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -953,9 +1381,15 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:spDef>
@@ -972,7 +1406,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
         <a:noAutofit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -991,7 +1425,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1017,7 +1451,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1043,7 +1477,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1069,7 +1503,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1095,7 +1529,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1121,7 +1555,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1147,7 +1581,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1173,7 +1607,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1199,7 +1633,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1225,7 +1659,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1238,9 +1672,15 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:lnDef>
@@ -1254,7 +1694,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1273,7 +1713,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1100" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1303,7 +1743,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1329,7 +1769,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1355,7 +1795,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1381,7 +1821,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1407,7 +1847,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1433,7 +1873,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1459,7 +1899,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1485,7 +1925,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1511,7 +1951,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1524,172 +1964,182 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:txDef>
   </a:objectDefaults>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I12"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
+    <sheetView showGridLines="0" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83333" defaultRowHeight="15" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.3516" style="1" customWidth="1"/>
-    <col min="2" max="2" width="16.4688" style="1" customWidth="1"/>
-    <col min="3" max="3" width="13.6719" style="1" customWidth="1"/>
-    <col min="4" max="4" width="35.1406" style="1" customWidth="1"/>
-    <col min="5" max="5" width="11.5" style="1" customWidth="1"/>
-    <col min="6" max="6" width="38.5" style="1" customWidth="1"/>
-    <col min="7" max="7" width="14.3516" style="1" customWidth="1"/>
-    <col min="8" max="8" width="22.5" style="1" customWidth="1"/>
+    <col min="1" max="1" width="10.33203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="16.44140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="13.6640625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="35.109375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="11.44140625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="38.44140625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="14.33203125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="22.44140625" style="1" customWidth="1"/>
     <col min="9" max="9" width="24" style="1" customWidth="1"/>
-    <col min="10" max="16384" width="8.85156" style="1" customWidth="1"/>
+    <col min="10" max="10" width="8.88671875" style="1" customWidth="1"/>
+    <col min="11" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="31.5" customHeight="1">
-      <c r="A1" t="s" s="2">
+    <row r="1" spans="1:9" ht="31.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s" s="3">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s" s="3">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s" s="3">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s" s="3">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s" s="4">
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="4" t="s">
         <v>5</v>
       </c>
       <c r="G1" s="5"/>
-      <c r="H1" t="s" s="4">
+      <c r="H1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="I1" t="s" s="6">
+      <c r="I1" s="6" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" ht="30" customHeight="1">
+    <row r="2" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="7">
         <v>1</v>
       </c>
-      <c r="B2" t="s" s="8">
+      <c r="B2" s="8" t="s">
         <v>7</v>
       </c>
       <c r="C2" s="9">
         <v>23</v>
       </c>
-      <c r="D2" t="s" s="8">
+      <c r="D2" s="8" t="s">
         <v>8</v>
       </c>
       <c r="E2" s="9">
         <v>0</v>
       </c>
-      <c r="F2" t="s" s="10">
+      <c r="F2" s="10" t="s">
         <v>9</v>
       </c>
       <c r="G2" s="5"/>
       <c r="H2" s="11">
         <v>1</v>
       </c>
-      <c r="I2" t="s" s="12">
+      <c r="I2" s="12" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="3" ht="45" customHeight="1">
+    <row r="3" spans="1:9" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="13">
         <v>2</v>
       </c>
-      <c r="B3" t="s" s="14">
+      <c r="B3" s="14" t="s">
         <v>11</v>
       </c>
       <c r="C3" s="15">
         <v>35</v>
       </c>
-      <c r="D3" t="s" s="14">
+      <c r="D3" s="14" t="s">
         <v>12</v>
       </c>
       <c r="E3" s="15">
         <v>7.99</v>
       </c>
-      <c r="F3" t="s" s="16">
+      <c r="F3" s="16" t="s">
         <v>13</v>
       </c>
       <c r="G3" s="17"/>
       <c r="H3" s="18">
         <v>2</v>
       </c>
-      <c r="I3" t="s" s="19">
+      <c r="I3" s="19" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="4" ht="31.5" customHeight="1">
+    <row r="4" spans="1:9" ht="31.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="7">
         <v>3</v>
       </c>
-      <c r="B4" t="s" s="8">
+      <c r="B4" s="8" t="s">
         <v>15</v>
       </c>
       <c r="C4" s="9">
         <v>20</v>
       </c>
-      <c r="D4" t="s" s="8">
+      <c r="D4" s="8" t="s">
         <v>16</v>
       </c>
       <c r="E4" s="9">
         <v>5.99</v>
       </c>
-      <c r="F4" t="s" s="10">
+      <c r="F4" s="10" t="s">
         <v>17</v>
       </c>
       <c r="G4" s="5"/>
       <c r="H4" s="11">
         <v>3</v>
       </c>
-      <c r="I4" t="s" s="12">
+      <c r="I4" s="12" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="5" ht="39" customHeight="1">
+    <row r="5" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="13">
         <v>4</v>
       </c>
-      <c r="B5" t="s" s="14">
+      <c r="B5" s="14" t="s">
         <v>19</v>
       </c>
       <c r="C5" s="15">
         <v>45</v>
       </c>
-      <c r="D5" t="s" s="14">
+      <c r="D5" s="14" t="s">
         <v>8</v>
       </c>
       <c r="E5" s="15">
         <v>0</v>
       </c>
-      <c r="F5" t="s" s="16">
+      <c r="F5" s="16" t="s">
         <v>20</v>
       </c>
       <c r="G5" s="17"/>
       <c r="H5" s="18">
         <v>4</v>
       </c>
-      <c r="I5" t="s" s="19">
+      <c r="I5" s="19" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="6" ht="38.1" customHeight="1">
+    <row r="6" spans="1:9" ht="38.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="20"/>
       <c r="B6" s="20"/>
       <c r="C6" s="20"/>
@@ -1700,17 +2150,17 @@
       <c r="H6" s="23"/>
       <c r="I6" s="23"/>
     </row>
-    <row r="7" ht="13.55" customHeight="1">
-      <c r="A7" t="s" s="2">
+    <row r="7" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B7" t="s" s="3">
+      <c r="B7" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C7" t="s" s="3">
+      <c r="C7" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="D7" t="s" s="3">
+      <c r="D7" s="3" t="s">
         <v>25</v>
       </c>
       <c r="E7" s="24"/>
@@ -1719,17 +2169,17 @@
       <c r="H7" s="22"/>
       <c r="I7" s="22"/>
     </row>
-    <row r="8" ht="26.55" customHeight="1">
+    <row r="8" spans="1:9" ht="26.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="7">
         <v>1</v>
       </c>
-      <c r="B8" t="s" s="8">
+      <c r="B8" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="C8" t="s" s="8">
+      <c r="C8" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="D8" t="s" s="26">
+      <c r="D8" s="26" t="s">
         <v>28</v>
       </c>
       <c r="E8" s="24"/>
@@ -1738,17 +2188,17 @@
       <c r="H8" s="22"/>
       <c r="I8" s="22"/>
     </row>
-    <row r="9" ht="13.55" customHeight="1">
+    <row r="9" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="13">
         <v>2</v>
       </c>
-      <c r="B9" t="s" s="14">
+      <c r="B9" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="C9" t="s" s="14">
+      <c r="C9" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="D9" t="s" s="27">
+      <c r="D9" s="27" t="s">
         <v>30</v>
       </c>
       <c r="E9" s="25"/>
@@ -1757,17 +2207,17 @@
       <c r="H9" s="22"/>
       <c r="I9" s="22"/>
     </row>
-    <row r="10" ht="26.55" customHeight="1">
+    <row r="10" spans="1:9" ht="26.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="7">
         <v>3</v>
       </c>
-      <c r="B10" t="s" s="8">
+      <c r="B10" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="C10" t="s" s="8">
+      <c r="C10" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="D10" t="s" s="26">
+      <c r="D10" s="26" t="s">
         <v>33</v>
       </c>
       <c r="E10" s="24"/>
@@ -1776,17 +2226,17 @@
       <c r="H10" s="22"/>
       <c r="I10" s="22"/>
     </row>
-    <row r="11" ht="39.55" customHeight="1">
+    <row r="11" spans="1:9" ht="39.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="13">
         <v>4</v>
       </c>
-      <c r="B11" t="s" s="14">
+      <c r="B11" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="C11" t="s" s="14">
+      <c r="C11" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="D11" t="s" s="27">
+      <c r="D11" s="27" t="s">
         <v>36</v>
       </c>
       <c r="E11" s="25"/>
@@ -1795,17 +2245,17 @@
       <c r="H11" s="22"/>
       <c r="I11" s="22"/>
     </row>
-    <row r="12" ht="26.55" customHeight="1">
+    <row r="12" spans="1:9" ht="26.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="7">
         <v>5</v>
       </c>
-      <c r="B12" t="s" s="8">
+      <c r="B12" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="C12" t="s" s="8">
+      <c r="C12" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="D12" t="s" s="26">
+      <c r="D12" s="26" t="s">
         <v>38</v>
       </c>
       <c r="E12" s="24"/>
@@ -1816,7 +2266,2456 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <pageSetup orientation="portrait"/>
+  <headerFooter>
+    <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J41"/>
+  <sheetViews>
+    <sheetView showGridLines="0" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="I13" sqref="I13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="10.33203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="18.44140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="17.88671875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="35.109375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="11.44140625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="38.44140625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="14.33203125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="22.44140625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="24" style="1" customWidth="1"/>
+    <col min="10" max="10" width="8.88671875" style="1" customWidth="1"/>
+    <col min="11" max="16384" width="8.88671875" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="40"/>
+      <c r="H1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="I1" s="58" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A2" s="7">
+        <v>1</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="9">
+        <v>23</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="9">
+        <v>0</v>
+      </c>
+      <c r="F2" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="G2" s="42"/>
+      <c r="H2" s="11">
+        <v>1</v>
+      </c>
+      <c r="I2" s="44" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A3" s="13">
+        <v>2</v>
+      </c>
+      <c r="B3" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="15">
+        <v>35</v>
+      </c>
+      <c r="D3" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="15">
+        <v>7.99</v>
+      </c>
+      <c r="F3" s="16" t="s">
+        <v>43</v>
+      </c>
+      <c r="G3" s="43"/>
+      <c r="H3" s="18">
+        <v>2</v>
+      </c>
+      <c r="I3" s="45" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A4" s="7">
+        <v>3</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="9">
+        <v>20</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" s="9">
+        <v>5.99</v>
+      </c>
+      <c r="F4" s="34" t="s">
+        <v>50</v>
+      </c>
+      <c r="G4" s="42"/>
+      <c r="H4" s="11">
+        <v>3</v>
+      </c>
+      <c r="I4" s="44" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A5" s="13">
+        <v>4</v>
+      </c>
+      <c r="B5" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" s="15">
+        <v>45</v>
+      </c>
+      <c r="D5" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" s="15">
+        <v>0</v>
+      </c>
+      <c r="F5" s="35" t="s">
+        <v>47</v>
+      </c>
+      <c r="G5" s="43"/>
+      <c r="H5" s="18">
+        <v>4</v>
+      </c>
+      <c r="I5" s="19" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A6" s="31">
+        <v>1</v>
+      </c>
+      <c r="B6" s="30" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="31">
+        <v>23</v>
+      </c>
+      <c r="D6" s="30" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6" s="31">
+        <v>0</v>
+      </c>
+      <c r="F6" s="32" t="s">
+        <v>39</v>
+      </c>
+      <c r="G6" s="42"/>
+      <c r="H6" s="11">
+        <v>1</v>
+      </c>
+      <c r="I6" s="44" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A7" s="28">
+        <v>1</v>
+      </c>
+      <c r="B7" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="15">
+        <v>23</v>
+      </c>
+      <c r="D7" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="E7" s="29">
+        <v>0</v>
+      </c>
+      <c r="F7" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="G7" s="42"/>
+      <c r="H7" s="18">
+        <v>1</v>
+      </c>
+      <c r="I7" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="J7" s="39"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A8" s="31">
+        <v>1</v>
+      </c>
+      <c r="B8" s="30" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="31">
+        <v>23</v>
+      </c>
+      <c r="D8" s="30" t="s">
+        <v>8</v>
+      </c>
+      <c r="E8" s="31">
+        <v>0</v>
+      </c>
+      <c r="F8" s="32" t="s">
+        <v>41</v>
+      </c>
+      <c r="G8" s="38"/>
+      <c r="H8" s="11">
+        <v>2</v>
+      </c>
+      <c r="I8" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="J8" s="39"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A9" s="13">
+        <v>2</v>
+      </c>
+      <c r="B9" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" s="15">
+        <v>35</v>
+      </c>
+      <c r="D9" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="E9" s="15">
+        <v>7.99</v>
+      </c>
+      <c r="F9" s="16" t="s">
+        <v>44</v>
+      </c>
+      <c r="G9" s="38"/>
+      <c r="H9" s="48">
+        <v>3</v>
+      </c>
+      <c r="I9" s="49" t="s">
+        <v>27</v>
+      </c>
+      <c r="J9" s="39"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A10" s="33">
+        <v>2</v>
+      </c>
+      <c r="B10" s="30" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" s="31">
+        <v>35</v>
+      </c>
+      <c r="D10" s="30" t="s">
+        <v>12</v>
+      </c>
+      <c r="E10" s="31">
+        <v>7.99</v>
+      </c>
+      <c r="F10" s="32" t="s">
+        <v>45</v>
+      </c>
+      <c r="G10" s="38"/>
+      <c r="H10" s="46"/>
+      <c r="I10" s="47"/>
+      <c r="J10" s="39"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A11" s="13">
+        <v>2</v>
+      </c>
+      <c r="B11" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" s="15">
+        <v>35</v>
+      </c>
+      <c r="D11" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="E11" s="15">
+        <v>7.99</v>
+      </c>
+      <c r="F11" s="16" t="s">
+        <v>46</v>
+      </c>
+      <c r="G11" s="38"/>
+      <c r="H11" s="46"/>
+      <c r="I11" s="47"/>
+      <c r="J11" s="39"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A12" s="33">
+        <v>4</v>
+      </c>
+      <c r="B12" s="30" t="s">
+        <v>19</v>
+      </c>
+      <c r="C12" s="31">
+        <v>45</v>
+      </c>
+      <c r="D12" s="30" t="s">
+        <v>8</v>
+      </c>
+      <c r="E12" s="31">
+        <v>0</v>
+      </c>
+      <c r="F12" s="32" t="s">
+        <v>47</v>
+      </c>
+      <c r="G12" s="38"/>
+      <c r="H12" s="46"/>
+      <c r="I12" s="47"/>
+      <c r="J12" s="39"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A13" s="13">
+        <v>4</v>
+      </c>
+      <c r="B13" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="C13" s="15">
+        <v>45</v>
+      </c>
+      <c r="D13" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="E13" s="15">
+        <v>0</v>
+      </c>
+      <c r="F13" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="G13" s="38"/>
+      <c r="H13" s="46"/>
+      <c r="I13" s="47"/>
+      <c r="J13" s="39"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A14" s="33">
+        <v>4</v>
+      </c>
+      <c r="B14" s="30" t="s">
+        <v>19</v>
+      </c>
+      <c r="C14" s="31">
+        <v>45</v>
+      </c>
+      <c r="D14" s="30" t="s">
+        <v>8</v>
+      </c>
+      <c r="E14" s="31">
+        <v>0</v>
+      </c>
+      <c r="F14" s="32" t="s">
+        <v>49</v>
+      </c>
+      <c r="G14" s="38"/>
+      <c r="H14" s="46"/>
+      <c r="I14" s="47"/>
+      <c r="J14" s="39"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A15" s="13">
+        <v>3</v>
+      </c>
+      <c r="B15" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="C15" s="15">
+        <v>20</v>
+      </c>
+      <c r="D15" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="E15" s="15">
+        <v>5.99</v>
+      </c>
+      <c r="F15" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="G15" s="38"/>
+      <c r="H15" s="46"/>
+      <c r="I15" s="47"/>
+      <c r="J15" s="39"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A16" s="33">
+        <v>3</v>
+      </c>
+      <c r="B16" s="30" t="s">
+        <v>15</v>
+      </c>
+      <c r="C16" s="31">
+        <v>20</v>
+      </c>
+      <c r="D16" s="30" t="s">
+        <v>16</v>
+      </c>
+      <c r="E16" s="31">
+        <v>5.99</v>
+      </c>
+      <c r="F16" s="32" t="s">
+        <v>39</v>
+      </c>
+      <c r="G16" s="38"/>
+      <c r="H16" s="46"/>
+      <c r="I16" s="47"/>
+      <c r="J16" s="39"/>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A17" s="13">
+        <v>4</v>
+      </c>
+      <c r="B17" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="C17" s="15">
+        <v>45</v>
+      </c>
+      <c r="D17" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="E17" s="15">
+        <v>0</v>
+      </c>
+      <c r="F17" s="35" t="s">
+        <v>48</v>
+      </c>
+      <c r="G17" s="38"/>
+      <c r="H17" s="46"/>
+      <c r="I17" s="47"/>
+      <c r="J17" s="39"/>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A18" s="33">
+        <v>4</v>
+      </c>
+      <c r="B18" s="30" t="s">
+        <v>19</v>
+      </c>
+      <c r="C18" s="31">
+        <v>45</v>
+      </c>
+      <c r="D18" s="30" t="s">
+        <v>8</v>
+      </c>
+      <c r="E18" s="31">
+        <v>0</v>
+      </c>
+      <c r="F18" s="36" t="s">
+        <v>49</v>
+      </c>
+      <c r="G18" s="38"/>
+      <c r="H18" s="46"/>
+      <c r="I18" s="47"/>
+      <c r="J18" s="39"/>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A19" s="50"/>
+      <c r="B19" s="51"/>
+      <c r="C19" s="50"/>
+      <c r="D19" s="51"/>
+      <c r="E19" s="50"/>
+      <c r="F19" s="52"/>
+      <c r="G19" s="38"/>
+      <c r="H19" s="46"/>
+      <c r="I19" s="47"/>
+      <c r="J19" s="39"/>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A20" s="53"/>
+      <c r="B20" s="54"/>
+      <c r="C20" s="53"/>
+      <c r="D20" s="54"/>
+      <c r="E20" s="53"/>
+      <c r="F20" s="47"/>
+      <c r="G20" s="38"/>
+      <c r="H20" s="46"/>
+      <c r="I20" s="47"/>
+      <c r="J20" s="39"/>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="E21" s="37"/>
+      <c r="F21" s="37"/>
+      <c r="G21" s="38"/>
+      <c r="H21" s="46"/>
+      <c r="I21" s="47"/>
+      <c r="J21" s="39"/>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="E22" s="37"/>
+      <c r="F22" s="37"/>
+      <c r="G22" s="38"/>
+      <c r="H22" s="38"/>
+      <c r="I22" s="38"/>
+      <c r="J22" s="39"/>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A23" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D23" s="73" t="s">
+        <v>60</v>
+      </c>
+      <c r="E23" s="37"/>
+      <c r="F23" s="37"/>
+      <c r="G23" s="38"/>
+      <c r="H23" s="38"/>
+      <c r="I23" s="38"/>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A24" s="7">
+        <v>1</v>
+      </c>
+      <c r="B24" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="C24" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="D24" s="34" t="s">
+        <v>42</v>
+      </c>
+      <c r="E24" s="37"/>
+      <c r="F24" s="37"/>
+      <c r="G24" s="38"/>
+      <c r="H24" s="38"/>
+      <c r="I24" s="38"/>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A25" s="13">
+        <v>2</v>
+      </c>
+      <c r="B25" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="C25" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="D25" s="35" t="s">
+        <v>50</v>
+      </c>
+      <c r="E25" s="37"/>
+      <c r="F25" s="37"/>
+      <c r="G25" s="38"/>
+      <c r="H25" s="38"/>
+      <c r="I25" s="38"/>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A26" s="7">
+        <v>3</v>
+      </c>
+      <c r="B26" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="C26" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="D26" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="E26" s="37"/>
+      <c r="F26" s="37"/>
+      <c r="G26" s="39"/>
+      <c r="H26" s="39"/>
+      <c r="I26" s="39"/>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A27" s="13">
+        <v>4</v>
+      </c>
+      <c r="B27" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="C27" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="D27" s="35" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A28" s="7">
+        <v>5</v>
+      </c>
+      <c r="B28" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="C28" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="D28" s="34" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A29" s="13">
+        <v>1</v>
+      </c>
+      <c r="B29" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="C29" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="D29" s="35" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A30" s="7">
+        <v>1</v>
+      </c>
+      <c r="B30" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="C30" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="D30" s="34" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A31" s="13">
+        <v>2</v>
+      </c>
+      <c r="B31" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="C31" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="D31" s="35" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A32" s="7">
+        <v>3</v>
+      </c>
+      <c r="B32" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="C32" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="D32" s="34" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A33" s="13">
+        <v>3</v>
+      </c>
+      <c r="B33" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="C33" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="D33" s="35" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A34" s="7">
+        <v>3</v>
+      </c>
+      <c r="B34" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="C34" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="D34" s="34" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A35" s="13">
+        <v>4</v>
+      </c>
+      <c r="B35" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="C35" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="D35" s="35" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A36" s="7">
+        <v>4</v>
+      </c>
+      <c r="B36" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="C36" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="D36" s="34" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A37" s="13">
+        <v>4</v>
+      </c>
+      <c r="B37" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="C37" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="D37" s="35" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A38" s="7">
+        <v>4</v>
+      </c>
+      <c r="B38" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="C38" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="D38" s="34" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A39" s="13">
+        <v>4</v>
+      </c>
+      <c r="B39" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="C39" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="D39" s="35" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A40" s="7">
+        <v>5</v>
+      </c>
+      <c r="B40" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="C40" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="D40" s="34" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A41" s="55">
+        <v>5</v>
+      </c>
+      <c r="B41" s="56" t="s">
+        <v>37</v>
+      </c>
+      <c r="C41" s="56" t="s">
+        <v>21</v>
+      </c>
+      <c r="D41" s="57" t="s">
+        <v>48</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <headerFooter>
+    <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J39"/>
+  <sheetViews>
+    <sheetView showGridLines="0" topLeftCell="B13" workbookViewId="0">
+      <selection activeCell="J4" sqref="J4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="10.33203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="16.88671875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="19" style="1" customWidth="1"/>
+    <col min="4" max="4" width="23.88671875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="38.44140625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="14.33203125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="15.44140625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="24" style="1" customWidth="1"/>
+    <col min="9" max="9" width="11.6640625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="28.33203125" style="1" customWidth="1"/>
+    <col min="11" max="16384" width="8.88671875" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="60" t="s">
+        <v>57</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="40"/>
+      <c r="G1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="H1" s="58" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A2" s="7">
+        <v>1</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="9">
+        <v>23</v>
+      </c>
+      <c r="D2" s="65">
+        <v>1</v>
+      </c>
+      <c r="E2" s="79">
+        <v>1</v>
+      </c>
+      <c r="F2" s="42"/>
+      <c r="G2" s="11">
+        <v>1</v>
+      </c>
+      <c r="H2" s="67">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A3" s="13">
+        <v>2</v>
+      </c>
+      <c r="B3" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="15">
+        <v>35</v>
+      </c>
+      <c r="D3" s="64">
+        <v>2</v>
+      </c>
+      <c r="E3" s="80">
+        <v>14</v>
+      </c>
+      <c r="F3" s="43"/>
+      <c r="G3" s="18">
+        <v>2</v>
+      </c>
+      <c r="H3" s="68">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A4" s="7">
+        <v>3</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="9">
+        <v>20</v>
+      </c>
+      <c r="D4" s="65">
+        <v>3</v>
+      </c>
+      <c r="E4" s="79">
+        <v>2</v>
+      </c>
+      <c r="F4" s="42"/>
+      <c r="G4" s="11">
+        <v>3</v>
+      </c>
+      <c r="H4" s="67">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A5" s="13">
+        <v>4</v>
+      </c>
+      <c r="B5" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" s="15">
+        <v>45</v>
+      </c>
+      <c r="D5" s="64">
+        <v>1</v>
+      </c>
+      <c r="E5" s="80">
+        <v>7</v>
+      </c>
+      <c r="F5" s="43"/>
+      <c r="G5" s="18">
+        <v>4</v>
+      </c>
+      <c r="H5" s="68">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A6" s="31">
+        <v>1</v>
+      </c>
+      <c r="B6" s="30" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="31">
+        <v>23</v>
+      </c>
+      <c r="D6" s="66">
+        <v>1</v>
+      </c>
+      <c r="E6" s="82">
+        <v>3</v>
+      </c>
+      <c r="F6" s="42"/>
+      <c r="G6" s="11">
+        <v>1</v>
+      </c>
+      <c r="H6" s="67">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A7" s="28">
+        <v>1</v>
+      </c>
+      <c r="B7" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="15">
+        <v>23</v>
+      </c>
+      <c r="D7" s="64">
+        <v>1</v>
+      </c>
+      <c r="E7" s="80">
+        <v>15</v>
+      </c>
+      <c r="F7" s="42"/>
+      <c r="G7" s="18">
+        <v>1</v>
+      </c>
+      <c r="H7" s="68">
+        <v>3</v>
+      </c>
+      <c r="I7" s="39"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A8" s="31">
+        <v>1</v>
+      </c>
+      <c r="B8" s="30" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="31">
+        <v>23</v>
+      </c>
+      <c r="D8" s="66">
+        <v>1</v>
+      </c>
+      <c r="E8" s="82">
+        <v>5</v>
+      </c>
+      <c r="F8" s="38"/>
+      <c r="G8" s="11">
+        <v>2</v>
+      </c>
+      <c r="H8" s="67">
+        <v>3</v>
+      </c>
+      <c r="I8" s="39"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A9" s="13">
+        <v>2</v>
+      </c>
+      <c r="B9" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" s="15">
+        <v>35</v>
+      </c>
+      <c r="D9" s="64">
+        <v>2</v>
+      </c>
+      <c r="E9" s="80">
+        <v>17</v>
+      </c>
+      <c r="F9" s="38"/>
+      <c r="G9" s="48">
+        <v>3</v>
+      </c>
+      <c r="H9" s="70">
+        <v>1</v>
+      </c>
+      <c r="I9" s="39"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A10" s="33">
+        <v>2</v>
+      </c>
+      <c r="B10" s="30" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" s="31">
+        <v>35</v>
+      </c>
+      <c r="D10" s="66">
+        <v>2</v>
+      </c>
+      <c r="E10" s="82">
+        <v>6</v>
+      </c>
+      <c r="F10" s="38"/>
+      <c r="G10" s="46"/>
+      <c r="H10" s="47"/>
+      <c r="I10" s="39"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A11" s="13">
+        <v>2</v>
+      </c>
+      <c r="B11" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" s="15">
+        <v>35</v>
+      </c>
+      <c r="D11" s="64">
+        <v>2</v>
+      </c>
+      <c r="E11" s="80">
+        <v>16</v>
+      </c>
+      <c r="F11" s="38"/>
+      <c r="G11" s="46"/>
+      <c r="H11" s="47"/>
+      <c r="I11" s="39"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A12" s="33">
+        <v>4</v>
+      </c>
+      <c r="B12" s="30" t="s">
+        <v>19</v>
+      </c>
+      <c r="C12" s="31">
+        <v>45</v>
+      </c>
+      <c r="D12" s="66">
+        <v>1</v>
+      </c>
+      <c r="E12" s="82">
+        <v>7</v>
+      </c>
+      <c r="F12" s="38"/>
+      <c r="G12" s="46"/>
+      <c r="H12" s="47"/>
+      <c r="I12" s="39"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A13" s="13">
+        <v>4</v>
+      </c>
+      <c r="B13" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="C13" s="15">
+        <v>45</v>
+      </c>
+      <c r="D13" s="64">
+        <v>1</v>
+      </c>
+      <c r="E13" s="80">
+        <v>18</v>
+      </c>
+      <c r="F13" s="38"/>
+      <c r="G13" s="59" t="s">
+        <v>57</v>
+      </c>
+      <c r="H13" s="58" t="s">
+        <v>3</v>
+      </c>
+      <c r="I13" s="58" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A14" s="33">
+        <v>4</v>
+      </c>
+      <c r="B14" s="30" t="s">
+        <v>19</v>
+      </c>
+      <c r="C14" s="31">
+        <v>45</v>
+      </c>
+      <c r="D14" s="66">
+        <v>1</v>
+      </c>
+      <c r="E14" s="82">
+        <v>12</v>
+      </c>
+      <c r="F14" s="38"/>
+      <c r="G14" s="11">
+        <v>1</v>
+      </c>
+      <c r="H14" s="44" t="s">
+        <v>8</v>
+      </c>
+      <c r="I14" s="67">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A15" s="13">
+        <v>3</v>
+      </c>
+      <c r="B15" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="C15" s="15">
+        <v>20</v>
+      </c>
+      <c r="D15" s="64">
+        <v>3</v>
+      </c>
+      <c r="E15" s="80">
+        <v>5</v>
+      </c>
+      <c r="F15" s="38"/>
+      <c r="G15" s="18">
+        <v>2</v>
+      </c>
+      <c r="H15" s="45" t="s">
+        <v>12</v>
+      </c>
+      <c r="I15" s="68">
+        <v>7.99</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A16" s="33">
+        <v>3</v>
+      </c>
+      <c r="B16" s="30" t="s">
+        <v>15</v>
+      </c>
+      <c r="C16" s="31">
+        <v>20</v>
+      </c>
+      <c r="D16" s="66">
+        <v>3</v>
+      </c>
+      <c r="E16" s="82">
+        <v>3</v>
+      </c>
+      <c r="F16" s="38"/>
+      <c r="G16" s="11">
+        <v>3</v>
+      </c>
+      <c r="H16" s="44" t="s">
+        <v>16</v>
+      </c>
+      <c r="I16" s="67">
+        <v>5.99</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A17" s="13">
+        <v>4</v>
+      </c>
+      <c r="B17" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="C17" s="15">
+        <v>45</v>
+      </c>
+      <c r="D17" s="64">
+        <v>1</v>
+      </c>
+      <c r="E17" s="80">
+        <v>18</v>
+      </c>
+      <c r="F17" s="38"/>
+      <c r="G17" s="41"/>
+      <c r="H17" s="63"/>
+      <c r="I17" s="39"/>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A18" s="33">
+        <v>4</v>
+      </c>
+      <c r="B18" s="30" t="s">
+        <v>19</v>
+      </c>
+      <c r="C18" s="31">
+        <v>45</v>
+      </c>
+      <c r="D18" s="66">
+        <v>1</v>
+      </c>
+      <c r="E18" s="82">
+        <v>12</v>
+      </c>
+      <c r="F18" s="38"/>
+      <c r="G18" s="46"/>
+      <c r="H18" s="61"/>
+      <c r="I18" s="39"/>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A19" s="53"/>
+      <c r="B19" s="54"/>
+      <c r="C19" s="53"/>
+      <c r="D19" s="54"/>
+      <c r="E19" s="61"/>
+      <c r="F19" s="62"/>
+      <c r="I19" s="39"/>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="E20" s="37"/>
+      <c r="I20" s="39"/>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A21" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C21" s="60" t="s">
+        <v>58</v>
+      </c>
+      <c r="D21" s="73" t="s">
+        <v>61</v>
+      </c>
+      <c r="E21" s="37"/>
+      <c r="F21" s="59" t="s">
+        <v>58</v>
+      </c>
+      <c r="G21" s="58" t="s">
+        <v>24</v>
+      </c>
+      <c r="I21" s="75" t="s">
+        <v>61</v>
+      </c>
+      <c r="J21" s="73" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A22" s="7">
+        <v>1</v>
+      </c>
+      <c r="B22" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="C22" s="65">
+        <v>1</v>
+      </c>
+      <c r="D22" s="79">
+        <v>1</v>
+      </c>
+      <c r="E22" s="37"/>
+      <c r="F22" s="11">
+        <v>1</v>
+      </c>
+      <c r="G22" s="44" t="s">
+        <v>27</v>
+      </c>
+      <c r="I22" s="76">
+        <v>1</v>
+      </c>
+      <c r="J22" s="34" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A23" s="13">
+        <v>2</v>
+      </c>
+      <c r="B23" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="C23" s="64">
+        <v>1</v>
+      </c>
+      <c r="D23" s="80">
+        <v>2</v>
+      </c>
+      <c r="E23" s="37"/>
+      <c r="F23" s="18">
+        <v>2</v>
+      </c>
+      <c r="G23" s="45" t="s">
+        <v>32</v>
+      </c>
+      <c r="I23" s="77">
+        <v>2</v>
+      </c>
+      <c r="J23" s="45" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A24" s="7">
+        <v>3</v>
+      </c>
+      <c r="B24" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="C24" s="65">
+        <v>2</v>
+      </c>
+      <c r="D24" s="79">
+        <v>3</v>
+      </c>
+      <c r="E24" s="37"/>
+      <c r="F24" s="11">
+        <v>3</v>
+      </c>
+      <c r="G24" s="44" t="s">
+        <v>35</v>
+      </c>
+      <c r="H24" s="61"/>
+      <c r="I24" s="76">
+        <v>3</v>
+      </c>
+      <c r="J24" s="34" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A25" s="13">
+        <v>4</v>
+      </c>
+      <c r="B25" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="C25" s="64">
+        <v>3</v>
+      </c>
+      <c r="D25" s="80">
+        <v>4</v>
+      </c>
+      <c r="F25" s="83">
+        <v>4</v>
+      </c>
+      <c r="G25" s="45" t="s">
+        <v>21</v>
+      </c>
+      <c r="H25" s="61"/>
+      <c r="I25" s="78">
+        <v>4</v>
+      </c>
+      <c r="J25" s="35" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A26" s="7">
+        <v>5</v>
+      </c>
+      <c r="B26" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="C26" s="65">
+        <v>4</v>
+      </c>
+      <c r="D26" s="79">
+        <v>5</v>
+      </c>
+      <c r="G26" s="46"/>
+      <c r="H26" s="61"/>
+      <c r="I26" s="76">
+        <v>5</v>
+      </c>
+      <c r="J26" s="34" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A27" s="13">
+        <v>1</v>
+      </c>
+      <c r="B27" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="C27" s="64">
+        <v>1</v>
+      </c>
+      <c r="D27" s="80">
+        <v>6</v>
+      </c>
+      <c r="G27" s="46"/>
+      <c r="H27" s="61"/>
+      <c r="I27" s="78">
+        <v>6</v>
+      </c>
+      <c r="J27" s="35" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A28" s="7">
+        <v>1</v>
+      </c>
+      <c r="B28" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="C28" s="65">
+        <v>1</v>
+      </c>
+      <c r="D28" s="79">
+        <v>7</v>
+      </c>
+      <c r="G28" s="46"/>
+      <c r="H28" s="61"/>
+      <c r="I28" s="76">
+        <v>7</v>
+      </c>
+      <c r="J28" s="34" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A29" s="13">
+        <v>2</v>
+      </c>
+      <c r="B29" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="C29" s="64">
+        <v>1</v>
+      </c>
+      <c r="D29" s="80">
+        <v>8</v>
+      </c>
+      <c r="G29" s="46"/>
+      <c r="H29" s="61"/>
+      <c r="I29" s="78">
+        <v>8</v>
+      </c>
+      <c r="J29" s="35" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A30" s="7">
+        <v>3</v>
+      </c>
+      <c r="B30" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="C30" s="65">
+        <v>2</v>
+      </c>
+      <c r="D30" s="79">
+        <v>9</v>
+      </c>
+      <c r="G30" s="46"/>
+      <c r="H30" s="61"/>
+      <c r="I30" s="76">
+        <v>9</v>
+      </c>
+      <c r="J30" s="34" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A31" s="13">
+        <v>3</v>
+      </c>
+      <c r="B31" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="C31" s="64">
+        <v>2</v>
+      </c>
+      <c r="D31" s="80">
+        <v>10</v>
+      </c>
+      <c r="G31" s="46"/>
+      <c r="H31" s="61"/>
+      <c r="I31" s="78">
+        <v>10</v>
+      </c>
+      <c r="J31" s="35" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A32" s="7">
+        <v>3</v>
+      </c>
+      <c r="B32" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="C32" s="65">
+        <v>2</v>
+      </c>
+      <c r="D32" s="79">
+        <v>11</v>
+      </c>
+      <c r="G32" s="46"/>
+      <c r="H32" s="61"/>
+      <c r="I32" s="76">
+        <v>11</v>
+      </c>
+      <c r="J32" s="34" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A33" s="13">
+        <v>4</v>
+      </c>
+      <c r="B33" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="C33" s="64">
+        <v>3</v>
+      </c>
+      <c r="D33" s="80">
+        <v>12</v>
+      </c>
+      <c r="I33" s="78">
+        <v>12</v>
+      </c>
+      <c r="J33" s="35" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A34" s="7">
+        <v>4</v>
+      </c>
+      <c r="B34" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="C34" s="65">
+        <v>3</v>
+      </c>
+      <c r="D34" s="79">
+        <v>13</v>
+      </c>
+      <c r="I34" s="76">
+        <v>13</v>
+      </c>
+      <c r="J34" s="34" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A35" s="13">
+        <v>4</v>
+      </c>
+      <c r="B35" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="C35" s="64">
+        <v>3</v>
+      </c>
+      <c r="D35" s="80">
+        <v>14</v>
+      </c>
+      <c r="I35" s="78">
+        <v>14</v>
+      </c>
+      <c r="J35" s="35" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A36" s="7">
+        <v>4</v>
+      </c>
+      <c r="B36" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="C36" s="65">
+        <v>3</v>
+      </c>
+      <c r="D36" s="79">
+        <v>15</v>
+      </c>
+      <c r="I36" s="76">
+        <v>15</v>
+      </c>
+      <c r="J36" s="34" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A37" s="13">
+        <v>4</v>
+      </c>
+      <c r="B37" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="C37" s="64">
+        <v>3</v>
+      </c>
+      <c r="D37" s="80">
+        <v>16</v>
+      </c>
+      <c r="I37" s="78">
+        <v>16</v>
+      </c>
+      <c r="J37" s="35" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A38" s="7">
+        <v>5</v>
+      </c>
+      <c r="B38" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="C38" s="65">
+        <v>4</v>
+      </c>
+      <c r="D38" s="79">
+        <v>17</v>
+      </c>
+      <c r="I38" s="76">
+        <v>17</v>
+      </c>
+      <c r="J38" s="34" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A39" s="55">
+        <v>5</v>
+      </c>
+      <c r="B39" s="56" t="s">
+        <v>37</v>
+      </c>
+      <c r="C39" s="71">
+        <v>4</v>
+      </c>
+      <c r="D39" s="81">
+        <v>18</v>
+      </c>
+      <c r="I39" s="78">
+        <v>18</v>
+      </c>
+      <c r="J39" s="57" t="s">
+        <v>48</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <headerFooter>
+    <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K54"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="9.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.88671875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="12.21875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="23.88671875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="4.44140625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="26.21875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="25.109375" style="1" customWidth="1"/>
+    <col min="8" max="8" width="24" style="1" customWidth="1"/>
+    <col min="9" max="9" width="4.44140625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="18" style="1" customWidth="1"/>
+    <col min="11" max="11" width="19.33203125" style="1" customWidth="1"/>
+    <col min="12" max="12" width="11.109375" style="1" customWidth="1"/>
+    <col min="13" max="16384" width="8.88671875" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="73" t="s">
+        <v>57</v>
+      </c>
+      <c r="E1" s="88"/>
+      <c r="F1" s="75" t="s">
+        <v>61</v>
+      </c>
+      <c r="G1" s="73" t="s">
+        <v>60</v>
+      </c>
+      <c r="H1" s="73" t="s">
+        <v>22</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="K1" s="58" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A2" s="7">
+        <v>1</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="9">
+        <v>23</v>
+      </c>
+      <c r="D2" s="74">
+        <v>1</v>
+      </c>
+      <c r="E2" s="84"/>
+      <c r="F2" s="76">
+        <v>1</v>
+      </c>
+      <c r="G2" s="34" t="s">
+        <v>42</v>
+      </c>
+      <c r="H2" s="86">
+        <v>1</v>
+      </c>
+      <c r="J2" s="7">
+        <v>1</v>
+      </c>
+      <c r="K2" s="79">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A3" s="13">
+        <v>2</v>
+      </c>
+      <c r="B3" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="15">
+        <v>35</v>
+      </c>
+      <c r="D3" s="85">
+        <v>2</v>
+      </c>
+      <c r="E3" s="84"/>
+      <c r="F3" s="77">
+        <v>2</v>
+      </c>
+      <c r="G3" s="45" t="s">
+        <v>50</v>
+      </c>
+      <c r="H3" s="87">
+        <v>2</v>
+      </c>
+      <c r="J3" s="13">
+        <v>2</v>
+      </c>
+      <c r="K3" s="80">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A4" s="7">
+        <v>3</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="9">
+        <v>20</v>
+      </c>
+      <c r="D4" s="74">
+        <v>3</v>
+      </c>
+      <c r="E4" s="84"/>
+      <c r="F4" s="76">
+        <v>3</v>
+      </c>
+      <c r="G4" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="H4" s="86">
+        <v>3</v>
+      </c>
+      <c r="J4" s="7">
+        <v>3</v>
+      </c>
+      <c r="K4" s="79">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A5" s="13">
+        <v>4</v>
+      </c>
+      <c r="B5" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" s="15">
+        <v>45</v>
+      </c>
+      <c r="D5" s="85">
+        <v>1</v>
+      </c>
+      <c r="E5" s="84"/>
+      <c r="F5" s="78">
+        <v>4</v>
+      </c>
+      <c r="G5" s="35" t="s">
+        <v>56</v>
+      </c>
+      <c r="H5" s="87">
+        <v>4</v>
+      </c>
+      <c r="J5" s="13">
+        <v>4</v>
+      </c>
+      <c r="K5" s="80">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A6" s="53"/>
+      <c r="B6" s="54"/>
+      <c r="C6" s="53"/>
+      <c r="D6" s="90"/>
+      <c r="E6" s="84"/>
+      <c r="F6" s="76">
+        <v>5</v>
+      </c>
+      <c r="G6" s="34" t="s">
+        <v>41</v>
+      </c>
+      <c r="H6" s="86">
+        <v>5</v>
+      </c>
+      <c r="J6" s="31">
+        <v>1</v>
+      </c>
+      <c r="K6" s="82">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A7" s="53"/>
+      <c r="B7" s="54"/>
+      <c r="C7" s="53"/>
+      <c r="D7" s="90"/>
+      <c r="E7" s="84"/>
+      <c r="F7" s="78">
+        <v>6</v>
+      </c>
+      <c r="G7" s="35" t="s">
+        <v>45</v>
+      </c>
+      <c r="H7" s="87">
+        <v>1</v>
+      </c>
+      <c r="I7" s="39"/>
+      <c r="J7" s="13">
+        <v>1</v>
+      </c>
+      <c r="K7" s="80">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" s="73" t="s">
+        <v>58</v>
+      </c>
+      <c r="D8" s="90"/>
+      <c r="E8" s="84"/>
+      <c r="F8" s="76">
+        <v>7</v>
+      </c>
+      <c r="G8" s="34" t="s">
+        <v>47</v>
+      </c>
+      <c r="H8" s="86">
+        <v>1</v>
+      </c>
+      <c r="I8" s="39"/>
+      <c r="J8" s="31">
+        <v>1</v>
+      </c>
+      <c r="K8" s="82">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A9" s="7">
+        <v>1</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="C9" s="74">
+        <v>1</v>
+      </c>
+      <c r="D9" s="90"/>
+      <c r="E9" s="84"/>
+      <c r="F9" s="78">
+        <v>8</v>
+      </c>
+      <c r="G9" s="35" t="s">
+        <v>51</v>
+      </c>
+      <c r="H9" s="87">
+        <v>2</v>
+      </c>
+      <c r="I9" s="39"/>
+      <c r="J9" s="13">
+        <v>2</v>
+      </c>
+      <c r="K9" s="80">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A10" s="13">
+        <v>2</v>
+      </c>
+      <c r="B10" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="C10" s="85">
+        <v>1</v>
+      </c>
+      <c r="D10" s="90"/>
+      <c r="E10" s="84"/>
+      <c r="F10" s="76">
+        <v>9</v>
+      </c>
+      <c r="G10" s="34" t="s">
+        <v>52</v>
+      </c>
+      <c r="H10" s="86">
+        <v>3</v>
+      </c>
+      <c r="I10" s="39"/>
+      <c r="J10" s="33">
+        <v>2</v>
+      </c>
+      <c r="K10" s="82">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A11" s="7">
+        <v>3</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="C11" s="74">
+        <v>2</v>
+      </c>
+      <c r="D11" s="90"/>
+      <c r="E11" s="84"/>
+      <c r="F11" s="78">
+        <v>10</v>
+      </c>
+      <c r="G11" s="35" t="s">
+        <v>53</v>
+      </c>
+      <c r="H11" s="87">
+        <v>3</v>
+      </c>
+      <c r="I11" s="39"/>
+      <c r="J11" s="13">
+        <v>2</v>
+      </c>
+      <c r="K11" s="80">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A12" s="13">
+        <v>4</v>
+      </c>
+      <c r="B12" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="C12" s="85">
+        <v>3</v>
+      </c>
+      <c r="D12" s="90"/>
+      <c r="F12" s="76">
+        <v>11</v>
+      </c>
+      <c r="G12" s="34" t="s">
+        <v>54</v>
+      </c>
+      <c r="H12" s="86">
+        <v>3</v>
+      </c>
+      <c r="I12" s="39"/>
+      <c r="J12" s="33">
+        <v>4</v>
+      </c>
+      <c r="K12" s="82">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A13" s="7">
+        <v>5</v>
+      </c>
+      <c r="B13" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="C13" s="74">
+        <v>4</v>
+      </c>
+      <c r="D13" s="90"/>
+      <c r="F13" s="78">
+        <v>12</v>
+      </c>
+      <c r="G13" s="35" t="s">
+        <v>49</v>
+      </c>
+      <c r="H13" s="87">
+        <v>4</v>
+      </c>
+      <c r="J13" s="13">
+        <v>3</v>
+      </c>
+      <c r="K13" s="80">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A14" s="53"/>
+      <c r="B14" s="54"/>
+      <c r="C14" s="53"/>
+      <c r="D14" s="90"/>
+      <c r="F14" s="76">
+        <v>13</v>
+      </c>
+      <c r="G14" s="34" t="s">
+        <v>55</v>
+      </c>
+      <c r="H14" s="86">
+        <v>4</v>
+      </c>
+      <c r="J14" s="33">
+        <v>3</v>
+      </c>
+      <c r="K14" s="82">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A15" s="53"/>
+      <c r="B15" s="54"/>
+      <c r="C15" s="53"/>
+      <c r="D15" s="90"/>
+      <c r="F15" s="78">
+        <v>14</v>
+      </c>
+      <c r="G15" s="35" t="s">
+        <v>43</v>
+      </c>
+      <c r="H15" s="87">
+        <v>4</v>
+      </c>
+      <c r="J15" s="13">
+        <v>4</v>
+      </c>
+      <c r="K15" s="80">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A16" s="59" t="s">
+        <v>58</v>
+      </c>
+      <c r="B16" s="58" t="s">
+        <v>24</v>
+      </c>
+      <c r="C16" s="53"/>
+      <c r="D16" s="90"/>
+      <c r="E16" s="84"/>
+      <c r="F16" s="76">
+        <v>15</v>
+      </c>
+      <c r="G16" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="H16" s="86">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A17" s="11">
+        <v>1</v>
+      </c>
+      <c r="B17" s="44" t="s">
+        <v>27</v>
+      </c>
+      <c r="C17" s="53"/>
+      <c r="D17" s="90"/>
+      <c r="F17" s="78">
+        <v>16</v>
+      </c>
+      <c r="G17" s="35" t="s">
+        <v>46</v>
+      </c>
+      <c r="H17" s="87">
+        <v>4</v>
+      </c>
+      <c r="I17" s="39"/>
+    </row>
+    <row r="18" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A18" s="18">
+        <v>2</v>
+      </c>
+      <c r="B18" s="45" t="s">
+        <v>32</v>
+      </c>
+      <c r="C18" s="53"/>
+      <c r="D18" s="90"/>
+      <c r="F18" s="76">
+        <v>17</v>
+      </c>
+      <c r="G18" s="34" t="s">
+        <v>44</v>
+      </c>
+      <c r="H18" s="86">
+        <v>5</v>
+      </c>
+      <c r="I18" s="39"/>
+      <c r="J18" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="K18" s="58" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A19" s="11">
+        <v>3</v>
+      </c>
+      <c r="B19" s="44" t="s">
+        <v>35</v>
+      </c>
+      <c r="C19" s="53"/>
+      <c r="D19" s="54"/>
+      <c r="F19" s="78">
+        <v>18</v>
+      </c>
+      <c r="G19" s="57" t="s">
+        <v>48</v>
+      </c>
+      <c r="H19" s="55">
+        <v>5</v>
+      </c>
+      <c r="I19" s="39"/>
+      <c r="J19" s="11">
+        <v>1</v>
+      </c>
+      <c r="K19" s="67">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A20" s="83">
+        <v>4</v>
+      </c>
+      <c r="B20" s="45" t="s">
+        <v>21</v>
+      </c>
+      <c r="I20" s="39"/>
+      <c r="J20" s="18">
+        <v>2</v>
+      </c>
+      <c r="K20" s="68">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="D21" s="72"/>
+      <c r="J21" s="11">
+        <v>3</v>
+      </c>
+      <c r="K21" s="67">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A22" s="59" t="s">
+        <v>57</v>
+      </c>
+      <c r="B22" s="58" t="s">
+        <v>3</v>
+      </c>
+      <c r="C22" s="58" t="s">
+        <v>4</v>
+      </c>
+      <c r="D22" s="84"/>
+      <c r="J22" s="18">
+        <v>4</v>
+      </c>
+      <c r="K22" s="68">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A23" s="69">
+        <v>1</v>
+      </c>
+      <c r="B23" s="44" t="s">
+        <v>8</v>
+      </c>
+      <c r="C23" s="67">
+        <v>0</v>
+      </c>
+      <c r="D23" s="84"/>
+      <c r="J23" s="11">
+        <v>1</v>
+      </c>
+      <c r="K23" s="67">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A24" s="89">
+        <v>2</v>
+      </c>
+      <c r="B24" s="45" t="s">
+        <v>12</v>
+      </c>
+      <c r="C24" s="68">
+        <v>7.99</v>
+      </c>
+      <c r="D24" s="84"/>
+      <c r="J24" s="18">
+        <v>1</v>
+      </c>
+      <c r="K24" s="68">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A25" s="69">
+        <v>3</v>
+      </c>
+      <c r="B25" s="44" t="s">
+        <v>16</v>
+      </c>
+      <c r="C25" s="67">
+        <v>5.99</v>
+      </c>
+      <c r="D25" s="84"/>
+      <c r="J25" s="11">
+        <v>2</v>
+      </c>
+      <c r="K25" s="67">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="D26" s="84"/>
+      <c r="J26" s="48">
+        <v>3</v>
+      </c>
+      <c r="K26" s="70">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A27" s="53"/>
+      <c r="B27" s="54"/>
+      <c r="C27" s="90"/>
+      <c r="D27" s="84"/>
+    </row>
+    <row r="28" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="C28" s="90"/>
+      <c r="D28" s="84"/>
+    </row>
+    <row r="29" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="C29" s="90"/>
+      <c r="D29" s="84"/>
+    </row>
+    <row r="30" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="C30" s="90"/>
+      <c r="D30" s="84"/>
+    </row>
+    <row r="31" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="C31" s="90"/>
+      <c r="D31" s="84"/>
+    </row>
+    <row r="32" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="C32" s="90"/>
+      <c r="D32" s="84"/>
+    </row>
+    <row r="33" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A33" s="53"/>
+      <c r="B33" s="54"/>
+      <c r="C33" s="90"/>
+      <c r="D33" s="84"/>
+    </row>
+    <row r="34" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A34" s="53"/>
+      <c r="B34" s="54"/>
+      <c r="C34" s="90"/>
+      <c r="D34" s="84"/>
+    </row>
+    <row r="35" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A35" s="53"/>
+      <c r="B35" s="54"/>
+      <c r="C35" s="90"/>
+      <c r="D35" s="84"/>
+    </row>
+    <row r="36" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A36" s="53"/>
+      <c r="B36" s="54"/>
+      <c r="C36" s="90"/>
+      <c r="D36" s="84"/>
+    </row>
+    <row r="37" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A37" s="53"/>
+      <c r="B37" s="54"/>
+      <c r="C37" s="90"/>
+      <c r="D37" s="84"/>
+    </row>
+    <row r="38" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A38" s="53"/>
+      <c r="B38" s="54"/>
+      <c r="C38" s="90"/>
+      <c r="D38" s="84"/>
+    </row>
+    <row r="39" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A39" s="53"/>
+      <c r="B39" s="54"/>
+      <c r="C39" s="90"/>
+      <c r="D39" s="84"/>
+    </row>
+    <row r="40" spans="1:4" ht="14.4" x14ac:dyDescent="0.3"/>
+    <row r="41" spans="1:4" ht="14.4" x14ac:dyDescent="0.3"/>
+    <row r="42" spans="1:4" ht="14.4" x14ac:dyDescent="0.3"/>
+    <row r="43" spans="1:4" ht="14.4" x14ac:dyDescent="0.3"/>
+    <row r="44" spans="1:4" ht="14.4" x14ac:dyDescent="0.3"/>
+    <row r="45" spans="1:4" ht="14.4" x14ac:dyDescent="0.3"/>
+    <row r="46" spans="1:4" ht="14.4" x14ac:dyDescent="0.3"/>
+    <row r="47" spans="1:4" ht="14.4" x14ac:dyDescent="0.3"/>
+    <row r="48" spans="1:4" ht="14.4" x14ac:dyDescent="0.3"/>
+    <row r="49" ht="14.4" x14ac:dyDescent="0.3"/>
+    <row r="50" ht="14.4" x14ac:dyDescent="0.3"/>
+    <row r="51" ht="14.4" x14ac:dyDescent="0.3"/>
+    <row r="52" ht="14.4" x14ac:dyDescent="0.3"/>
+    <row r="53" ht="14.4" x14ac:dyDescent="0.3"/>
+    <row r="54" ht="14.4" x14ac:dyDescent="0.3"/>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>

</xml_diff>